<commit_message>
Aktualizace na spravny share
</commit_message>
<xml_diff>
--- a/Shareholding_EL-VY.xlsx
+++ b/Shareholding_EL-VY.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vytahy-my.sharepoint.com/personal/jan_holec_el-vy_cz/Documents/Dokumenty/__EL-VY/_RIZENI FIRMY/_System firmy/Shareholding_EL-VY/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_F6E04B4D5FB21028D5AE2537CC2528E350C270A7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECCAF103-1CFE-4B6B-837E-6CD65D616E89}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="11_F6E04B4D5FB21028D5AE2537CC2528E350C270A7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{017F65C6-D1E5-4200-BE17-CEE41B749384}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="List 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Share_prog" sheetId="1" r:id="rId1"/>
+    <sheet name="Seznam jmen" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="85">
   <si>
     <t>Priklad realizace Shareholdingu se zamestnanci EL-VY</t>
   </si>
@@ -228,6 +229,66 @@
   </si>
   <si>
     <t>Počet ŘADOVÝCH zaměstnanců</t>
+  </si>
+  <si>
+    <t>Shareholding za jeden rok</t>
+  </si>
+  <si>
+    <t>Shareholding po věrnostním období</t>
+  </si>
+  <si>
+    <t>Experimentalni, uvaha jestli vůbec a když tak jak…</t>
+  </si>
+  <si>
+    <t>Klicovy zamestnanci</t>
+  </si>
+  <si>
+    <t>Duleziti z.</t>
+  </si>
+  <si>
+    <t>Strategicky z.</t>
+  </si>
+  <si>
+    <t>Obchdonici</t>
+  </si>
+  <si>
+    <t>Mareckova</t>
+  </si>
+  <si>
+    <t>Kalny</t>
+  </si>
+  <si>
+    <t>Rakusan</t>
+  </si>
+  <si>
+    <t>Neruda</t>
+  </si>
+  <si>
+    <t>Malek Vl.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soudek </t>
+  </si>
+  <si>
+    <t>Lhotsky</t>
+  </si>
+  <si>
+    <t>Denk</t>
+  </si>
+  <si>
+    <t>Hochman</t>
+  </si>
+  <si>
+    <t>Meduna T.</t>
+  </si>
+  <si>
+    <t>Moucka ml.</t>
+  </si>
+  <si>
+    <t>Drnec</t>
+  </si>
+  <si>
+    <t>Procenta pro spolecniky z celkoveho zisku</t>
   </si>
 </sst>
 </file>
@@ -334,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -370,6 +431,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -588,15 +650,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z102"/>
+  <dimension ref="A1:Z106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
@@ -706,7 +768,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
@@ -714,7 +776,7 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -722,7 +784,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -730,7 +792,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -738,13 +800,13 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C22" s="2">
         <f>C18*C21</f>
         <v>200000</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -755,7 +817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>12</v>
       </c>
@@ -767,7 +829,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -782,7 +844,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -794,7 +856,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
@@ -809,7 +871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
@@ -818,7 +880,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>17</v>
       </c>
@@ -830,89 +892,36 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
+    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="4">
+        <f>D26</f>
+        <v>40000</v>
+      </c>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="4">
+        <f>C31*C24</f>
+        <v>200000</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="34" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="10">
+      <c r="C34" s="10">
         <v>0.01</v>
-      </c>
-      <c r="D32" s="11">
-        <f>C18*C32</f>
-        <v>40000</v>
-      </c>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
-      <c r="R32" s="9"/>
-      <c r="S32" s="9"/>
-      <c r="T32" s="9"/>
-      <c r="U32" s="9"/>
-      <c r="V32" s="9"/>
-      <c r="W32" s="9"/>
-      <c r="X32" s="9"/>
-      <c r="Y32" s="9"/>
-      <c r="Z32" s="9"/>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="13">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="D33" s="14">
-        <f>C18*C33</f>
-        <v>28000</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
-      <c r="R33" s="9"/>
-      <c r="S33" s="9"/>
-      <c r="T33" s="9"/>
-      <c r="U33" s="9"/>
-      <c r="V33" s="9"/>
-      <c r="W33" s="9"/>
-      <c r="X33" s="9"/>
-      <c r="Y33" s="9"/>
-      <c r="Z33" s="9"/>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A34" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="13">
-        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D34" s="11">
         <f>C18*C34</f>
-        <v>12000</v>
+        <v>40000</v>
       </c>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
@@ -937,20 +946,20 @@
       <c r="Y34" s="9"/>
       <c r="Z34" s="9"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B35" s="9"/>
-      <c r="C35" s="16">
-        <v>12</v>
+      <c r="C35" s="13">
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="D35" s="14">
-        <f>D34/C35</f>
-        <v>1000</v>
+        <f>C18*C35</f>
+        <v>28000</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
@@ -974,16 +983,18 @@
       <c r="Y35" s="9"/>
       <c r="Z35" s="9"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A36" s="12" t="s">
-        <v>16</v>
+    <row r="36" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="B36" s="9"/>
-      <c r="C36" s="11">
-        <f>D33*C24</f>
-        <v>140000</v>
-      </c>
-      <c r="D36" s="9"/>
+      <c r="C36" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D36" s="11">
+        <f>C18*C36</f>
+        <v>12000</v>
+      </c>
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
@@ -1007,19 +1018,21 @@
       <c r="Y36" s="9"/>
       <c r="Z36" s="9"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B37" s="9"/>
-      <c r="C37" s="11">
-        <f>(D33+D34)*C24</f>
-        <v>200000</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" s="9"/>
+      <c r="C37" s="16">
+        <v>12</v>
+      </c>
+      <c r="D37" s="14">
+        <f>D36/C37</f>
+        <v>1000</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>15</v>
+      </c>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -1042,518 +1055,740 @@
       <c r="Y37" s="9"/>
       <c r="Z37" s="9"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="11">
+        <f>D35*C24</f>
+        <v>140000</v>
+      </c>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
+      <c r="R38" s="9"/>
+      <c r="S38" s="9"/>
+      <c r="T38" s="9"/>
+      <c r="U38" s="9"/>
+      <c r="V38" s="9"/>
+      <c r="W38" s="9"/>
+      <c r="X38" s="9"/>
+      <c r="Y38" s="9"/>
+      <c r="Z38" s="9"/>
+    </row>
+    <row r="39" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="11">
+        <f>(D35+D36)*C24</f>
+        <v>200000</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
+      <c r="R39" s="9"/>
+      <c r="S39" s="9"/>
+      <c r="T39" s="9"/>
+      <c r="U39" s="9"/>
+      <c r="V39" s="9"/>
+      <c r="W39" s="9"/>
+      <c r="X39" s="9"/>
+      <c r="Y39" s="9"/>
+      <c r="Z39" s="9"/>
+    </row>
+    <row r="40" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="4">
+        <f>D35</f>
+        <v>28000</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
+      <c r="R40" s="9"/>
+      <c r="S40" s="9"/>
+      <c r="T40" s="9"/>
+      <c r="U40" s="9"/>
+      <c r="V40" s="9"/>
+      <c r="W40" s="9"/>
+      <c r="X40" s="9"/>
+      <c r="Y40" s="9"/>
+      <c r="Z40" s="9"/>
+    </row>
+    <row r="41" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C41" s="4">
+        <f>C24*C40</f>
+        <v>140000</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="9"/>
+      <c r="R41" s="9"/>
+      <c r="S41" s="9"/>
+      <c r="T41" s="9"/>
+      <c r="U41" s="9"/>
+      <c r="V41" s="9"/>
+      <c r="W41" s="9"/>
+      <c r="X41" s="9"/>
+      <c r="Y41" s="9"/>
+      <c r="Z41" s="9"/>
+    </row>
+    <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="9"/>
+    </row>
+    <row r="44" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="17">
-        <v>5</v>
-      </c>
-      <c r="D40" s="18">
-        <f>C40*C30</f>
-        <v>2500000</v>
-      </c>
-      <c r="E40" s="1" t="s">
+      <c r="C44" s="17">
+        <v>4</v>
+      </c>
+      <c r="D44" s="18">
+        <f>C44*C32</f>
+        <v>800000</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+    <row r="45" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="1">
-        <f>C40</f>
-        <v>5</v>
-      </c>
-      <c r="D41" s="18">
-        <f>D40/C24</f>
-        <v>500000</v>
-      </c>
-      <c r="E41" s="1" t="s">
+      <c r="C45" s="1">
+        <f>C44</f>
+        <v>4</v>
+      </c>
+      <c r="D45" s="18">
+        <f>D44/C24</f>
+        <v>160000</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="46" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="17">
-        <v>3</v>
-      </c>
-      <c r="D42" s="18">
-        <f>C42*C37</f>
-        <v>600000</v>
-      </c>
-      <c r="E42" s="1" t="s">
+      <c r="C46" s="17">
+        <v>4</v>
+      </c>
+      <c r="D46" s="18">
+        <f>C46*C41</f>
+        <v>560000</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+    <row r="47" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C43" s="1">
-        <f>C42</f>
-        <v>3</v>
-      </c>
-      <c r="D43" s="18">
-        <f>D42/C24</f>
-        <v>120000</v>
-      </c>
-      <c r="E43" s="1" t="s">
+      <c r="C47" s="1">
+        <f>C46</f>
+        <v>4</v>
+      </c>
+      <c r="D47" s="18">
+        <f>D46/C24</f>
+        <v>112000</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+    <row r="48" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+    <row r="50" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C50" s="4">
         <f>C24*(C18-C20-C22)</f>
         <v>14000000</v>
       </c>
-      <c r="D46" s="4">
-        <f>C46-D40-D42-D74-D84-D102</f>
-        <v>6300000</v>
-      </c>
-      <c r="E46" s="19">
-        <f>100-(100*D46/C46)</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A47" s="19" t="s">
+      <c r="D50" s="4">
+        <f>C50-D44-D46-D78-D88-D106</f>
+        <v>7572000</v>
+      </c>
+      <c r="E50" s="19">
+        <f>100-(100*D50/C50)</f>
+        <v>45.914285714285711</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A51" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="4">
-        <f t="shared" ref="C47:D47" si="0">0.6*C46</f>
+      <c r="C51" s="4">
+        <f t="shared" ref="C51:D51" si="0">0.6*C50</f>
         <v>8400000</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D51" s="4">
         <f t="shared" si="0"/>
-        <v>3780000</v>
-      </c>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A48" s="19" t="s">
+        <v>4543200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A52" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="4">
-        <f t="shared" ref="C48:D48" si="1">0.2*C46</f>
+      <c r="C52" s="4">
+        <f t="shared" ref="C52:D52" si="1">0.2*C50</f>
         <v>2800000</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D52" s="4">
         <f t="shared" si="1"/>
-        <v>1260000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="19" t="s">
+        <v>1514400</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C49" s="4">
-        <f t="shared" ref="C49:D49" si="2">0.2*C46</f>
+      <c r="C53" s="4">
+        <f t="shared" ref="C53:D53" si="2">0.2*C50</f>
         <v>2800000</v>
       </c>
-      <c r="D49" s="4">
+      <c r="D53" s="4">
         <f t="shared" si="2"/>
-        <v>1260000</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+        <v>1514400</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C52" s="4">
+      <c r="C56" s="4">
         <f>(C18-C20-C22)</f>
         <v>2800000</v>
       </c>
-      <c r="D52" s="4">
-        <f>C52-D41-D43-D73-D83-D101</f>
-        <v>1560000</v>
-      </c>
-      <c r="E52" s="20">
-        <f>100-(100*D52/C18)</f>
-        <v>61</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+      <c r="D56" s="4">
+        <f>C56-D57</f>
+        <v>2408000</v>
+      </c>
+      <c r="E56" s="20">
+        <f>100-(100*D56/C18)</f>
+        <v>39.799999999999997</v>
+      </c>
+      <c r="F56" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D53" s="4">
-        <f>D41+D43+D73+D83+D101</f>
-        <v>1240000</v>
-      </c>
-      <c r="E53" s="21">
-        <f>(100*D53/C18)</f>
-        <v>31</v>
-      </c>
-      <c r="F53" s="1" t="s">
+      <c r="D57" s="4">
+        <f>D45+D47+D87</f>
+        <v>392000</v>
+      </c>
+      <c r="E57" s="21">
+        <f>(100*D57/C18)</f>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F57" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D58" s="25"/>
+    </row>
+    <row r="59" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="7" t="s">
+    <row r="61" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A61" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+    <row r="62" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C62" s="1">
         <v>5</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D62" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
+    <row r="63" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+    <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4">
-        <v>5000000</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1">
-        <v>10</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="4">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1">
+        <v>10</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4">
         <v>200000</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B65" s="1" t="s">
+    <row r="69" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B69" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B70" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C65" s="22"/>
-      <c r="D65" s="22">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B66" s="1" t="s">
+      <c r="D70" s="4">
+        <f>D68*(1-D69)</f>
+        <v>160000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B71" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D66" s="4">
-        <f>D64*(1-D65)</f>
+      <c r="C71" s="23"/>
+      <c r="D71" s="23">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B72" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C72" s="6"/>
+      <c r="D72" s="2">
+        <f>D70*D71</f>
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C74" s="6"/>
+      <c r="D74" s="2">
+        <f>D72*D65</f>
         <v>160000</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B67" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C67" s="23"/>
-      <c r="D67" s="23">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B68" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C68" s="6"/>
-      <c r="D68" s="2">
-        <f>D66*D67</f>
-        <v>16000</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C70" s="6"/>
-      <c r="D70" s="2">
-        <f>D68*D61</f>
-        <v>160000</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
+    <row r="76" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D72" s="1">
+      <c r="D76" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A73" s="6" t="s">
+    <row r="77" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A77" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D73" s="18">
-        <f>D70*D72</f>
+      <c r="D77" s="18">
+        <f>D74*D76</f>
         <v>320000</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A74" s="6" t="s">
+    <row r="78" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A78" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D74" s="18">
-        <f>D73*C58</f>
+      <c r="D78" s="18">
+        <f>D77*C62</f>
         <v>1600000</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="E78" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A76" s="7" t="s">
+    <row r="80" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A80" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
+    <row r="81" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C81" s="1">
         <v>5</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A78" s="1" t="s">
+    <row r="82" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C78" s="3">
+      <c r="C82" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D78" s="4">
-        <f>C18*C78</f>
+      <c r="D82" s="4">
+        <f>C18*C82</f>
         <v>60000</v>
       </c>
-      <c r="E78" s="6" t="s">
+      <c r="E82" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
+    <row r="83" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D79" s="4">
-        <f>D78*C77</f>
+      <c r="D83" s="4">
+        <f>D82*C81</f>
         <v>300000</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
+    <row r="84" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D80" s="4">
-        <f>C77*D78+D79</f>
+      <c r="D84" s="4">
+        <f>C81*D82+D83</f>
         <v>600000</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="1" t="s">
+    <row r="86" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D82" s="1">
+      <c r="D86" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="6" t="s">
+    <row r="87" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A87" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D83" s="18">
-        <f>D78*D82</f>
+      <c r="D87" s="18">
+        <f>D82*D86</f>
         <v>120000</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="6" t="s">
+    <row r="88" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A88" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D84" s="18">
-        <f>(D78*C77+D79)*D82</f>
+      <c r="D88" s="18">
+        <f>(D82*C81+D83)*D86</f>
         <v>1200000</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="7" t="s">
+    <row r="90" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A90" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="1" t="s">
+    <row r="91" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C87" s="1">
+      <c r="C91" s="1">
         <v>5</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D91" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" s="1" t="s">
+    <row r="92" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D88" s="4">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" s="1" t="s">
+      <c r="D92" s="4">
+        <v>42000</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D89" s="4">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" s="1" t="s">
+      <c r="D93" s="4">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D90" s="3">
+      <c r="D94" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" s="1" t="s">
+    <row r="95" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D91" s="2">
-        <f>D88*D90</f>
-        <v>750</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" s="1" t="s">
+      <c r="D95" s="2">
+        <f>D92*D94</f>
+        <v>630</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C93" s="1">
+      <c r="C97" s="1">
         <v>5</v>
       </c>
-      <c r="D93" s="4">
-        <f>$D89+$D91*C93</f>
-        <v>33750</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C94" s="1">
+      <c r="D97" s="4">
+        <f>$D93+$D95*C97</f>
+        <v>29150</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C98" s="1">
         <v>10</v>
       </c>
-      <c r="D94" s="4">
-        <f>D89+D91*C94</f>
-        <v>37500</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C95" s="1">
+      <c r="D98" s="4">
+        <f>D93+D95*C98</f>
+        <v>32300</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C99" s="1">
         <v>15</v>
       </c>
-      <c r="D95" s="4">
-        <f>D89+D91*C95</f>
-        <v>41250</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
+      <c r="D99" s="4">
+        <f>D93+D95*C99</f>
+        <v>35450</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C97" s="1">
+      <c r="C101" s="1">
         <v>12</v>
       </c>
-      <c r="D97" s="2">
-        <f>C87*D91*C97</f>
-        <v>45000</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
+      <c r="D101" s="2">
+        <f>C91*D95*C101</f>
+        <v>37800</v>
+      </c>
+      <c r="E101" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D99" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" s="6" t="s">
+      <c r="D103" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A105" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D101" s="18">
-        <f>D99*C97*D91</f>
-        <v>180000</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" s="6" t="s">
+      <c r="D105" s="18">
+        <f>D103*C101*D95</f>
+        <v>226800</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="17.25" x14ac:dyDescent="0.4">
+      <c r="A106" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D102" s="24">
-        <f>D99*C97*D91*C87+D97*D99</f>
-        <v>1800000</v>
+      <c r="D106" s="24">
+        <f>D103*C101*D95*C91+D101*D103</f>
+        <v>2268000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{062C0369-ECBF-4FBB-9BB0-E17A56F48A53}">
+  <dimension ref="A2:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Priklad promenne dle pojmenovani bunky
Ve formule lze pouzit jmeno bunky namisto jejiho pismena a cisla (souradnice). Priklad: C18 se jmenuje HosVysl2021 a je pouzita pro vypocet E57.
</commit_message>
<xml_diff>
--- a/Shareholding_EL-VY.xlsx
+++ b/Shareholding_EL-VY.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vytahy-my.sharepoint.com/personal/jan_holec_el-vy_cz/Documents/Dokumenty/__EL-VY/_RIZENI FIRMY/_System firmy/Shareholding_EL-VY/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/holec1/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="11_F6E04B4D5FB21028D5AE2537CC2528E350C270A7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{017F65C6-D1E5-4200-BE17-CEE41B749384}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B4A992A-5C90-5344-AA9C-9E8F087FBB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Share_prog" sheetId="1" r:id="rId1"/>
     <sheet name="Seznam jmen" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="HosVysl2021">Share_prog!$C$18</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -295,9 +298,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0\ [$Kč-405]"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00\ [$Kč-405]"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -427,14 +431,14 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -652,24 +656,24 @@
   </sheetPr>
   <dimension ref="A1:Z106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="43.140625" customWidth="1"/>
+    <col min="2" max="2" width="43.1640625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -677,7 +681,7 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -685,7 +689,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -693,7 +697,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -701,13 +705,13 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="C7" s="2">
         <f>C3*C6</f>
         <v>200000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -719,7 +723,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -731,7 +735,7 @@
         <v>56000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -743,7 +747,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -754,7 +758,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -763,12 +767,12 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
@@ -776,7 +780,7 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -784,7 +788,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -792,7 +796,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -800,13 +804,13 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="C22" s="2">
         <f>C18*C21</f>
         <v>200000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -817,7 +821,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A25" s="7" t="s">
         <v>12</v>
       </c>
@@ -829,7 +833,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -844,7 +848,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -856,7 +860,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
@@ -871,7 +875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
@@ -880,7 +884,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>17</v>
       </c>
@@ -892,7 +896,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
@@ -902,7 +906,7 @@
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>66</v>
       </c>
@@ -912,7 +916,7 @@
       </c>
       <c r="D32" s="1"/>
     </row>
-    <row r="34" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="8" t="s">
         <v>19</v>
       </c>
@@ -946,7 +950,7 @@
       <c r="Y34" s="9"/>
       <c r="Z34" s="9"/>
     </row>
-    <row r="35" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A35" s="12" t="s">
         <v>6</v>
       </c>
@@ -983,7 +987,7 @@
       <c r="Y35" s="9"/>
       <c r="Z35" s="9"/>
     </row>
-    <row r="36" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="9" t="s">
         <v>7</v>
       </c>
@@ -1018,7 +1022,7 @@
       <c r="Y36" s="9"/>
       <c r="Z36" s="9"/>
     </row>
-    <row r="37" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A37" s="12" t="s">
         <v>14</v>
       </c>
@@ -1055,7 +1059,7 @@
       <c r="Y37" s="9"/>
       <c r="Z37" s="9"/>
     </row>
-    <row r="38" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A38" s="12" t="s">
         <v>16</v>
       </c>
@@ -1088,7 +1092,7 @@
       <c r="Y38" s="9"/>
       <c r="Z38" s="9"/>
     </row>
-    <row r="39" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="12" t="s">
         <v>17</v>
       </c>
@@ -1123,7 +1127,7 @@
       <c r="Y39" s="9"/>
       <c r="Z39" s="9"/>
     </row>
-    <row r="40" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>65</v>
       </c>
@@ -1155,7 +1159,7 @@
       <c r="Y40" s="9"/>
       <c r="Z40" s="9"/>
     </row>
-    <row r="41" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>66</v>
       </c>
@@ -1187,10 +1191,10 @@
       <c r="Y41" s="9"/>
       <c r="Z41" s="9"/>
     </row>
-    <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="9"/>
     </row>
-    <row r="44" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>20</v>
       </c>
@@ -1205,7 +1209,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>20</v>
       </c>
@@ -1221,7 +1225,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>23</v>
       </c>
@@ -1236,7 +1240,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>23</v>
       </c>
@@ -1252,10 +1256,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>24</v>
       </c>
@@ -1269,7 +1273,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>28</v>
       </c>
@@ -1286,7 +1290,7 @@
         <v>45.914285714285711</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="19" t="s">
         <v>29</v>
       </c>
@@ -1299,7 +1303,7 @@
         <v>4543200</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="19" t="s">
         <v>30</v>
       </c>
@@ -1312,7 +1316,7 @@
         <v>1514400</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="19" t="s">
         <v>31</v>
       </c>
@@ -1325,7 +1329,7 @@
         <v>1514400</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>32</v>
       </c>
@@ -1337,7 +1341,7 @@
       </c>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
         <v>28</v>
       </c>
@@ -1357,7 +1361,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>33</v>
       </c>
@@ -1365,28 +1369,28 @@
         <f>D45+D47+D87</f>
         <v>392000</v>
       </c>
-      <c r="E57" s="21">
-        <f>(100*D57/C18)</f>
+      <c r="E57" s="25">
+        <f>(100*D57/HosVysl2021)</f>
         <v>9.8000000000000007</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D58" s="25"/>
-    </row>
-    <row r="59" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D58" s="24"/>
+    </row>
+    <row r="59" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
         <v>37</v>
       </c>
@@ -1397,12 +1401,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
         <v>39</v>
       </c>
@@ -1411,7 +1415,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
         <v>40</v>
       </c>
@@ -1423,12 +1427,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
         <v>43</v>
       </c>
@@ -1437,16 +1441,16 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="B69" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C69" s="22"/>
-      <c r="D69" s="22">
+      <c r="C69" s="21"/>
+      <c r="D69" s="21">
         <v>0.2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="B70" s="1" t="s">
         <v>45</v>
       </c>
@@ -1455,16 +1459,16 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="B71" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C71" s="23"/>
-      <c r="D71" s="23">
+      <c r="C71" s="22"/>
+      <c r="D71" s="22">
         <v>0.1</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="B72" s="1" t="s">
         <v>47</v>
       </c>
@@ -1474,12 +1478,12 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B73" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
         <v>49</v>
       </c>
@@ -1489,7 +1493,7 @@
         <v>160000</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
         <v>50</v>
       </c>
@@ -1497,7 +1501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A77" s="6" t="s">
         <v>51</v>
       </c>
@@ -1506,7 +1510,7 @@
         <v>320000</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A78" s="6" t="s">
         <v>52</v>
       </c>
@@ -1518,12 +1522,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A80" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
         <v>8</v>
       </c>
@@ -1534,7 +1538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
         <v>55</v>
       </c>
@@ -1549,7 +1553,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
         <v>16</v>
       </c>
@@ -1558,7 +1562,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
         <v>17</v>
       </c>
@@ -1567,7 +1571,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
         <v>56</v>
       </c>
@@ -1575,7 +1579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="6" t="s">
         <v>51</v>
       </c>
@@ -1584,7 +1588,7 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="6" t="s">
         <v>52</v>
       </c>
@@ -1593,12 +1597,12 @@
         <v>1200000</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
         <v>8</v>
       </c>
@@ -1609,7 +1613,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
         <v>58</v>
       </c>
@@ -1617,7 +1621,7 @@
         <v>42000</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
         <v>59</v>
       </c>
@@ -1625,7 +1629,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
         <v>60</v>
       </c>
@@ -1633,7 +1637,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
         <v>61</v>
       </c>
@@ -1642,7 +1646,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
         <v>62</v>
       </c>
@@ -1654,7 +1658,7 @@
         <v>29150</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="C98" s="1">
         <v>10</v>
       </c>
@@ -1663,7 +1667,7 @@
         <v>32300</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="C99" s="1">
         <v>15</v>
       </c>
@@ -1672,7 +1676,7 @@
         <v>35450</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
         <v>63</v>
       </c>
@@ -1687,7 +1691,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A103" s="1" t="s">
         <v>64</v>
       </c>
@@ -1695,7 +1699,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A105" s="6" t="s">
         <v>51</v>
       </c>
@@ -1704,11 +1708,11 @@
         <v>226800</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="17.25" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:5" ht="14" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D106" s="24">
+      <c r="D106" s="23">
         <f>D103*C101*D95*C91+D101*D103</f>
         <v>2268000</v>
       </c>
@@ -1726,14 +1730,14 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -1747,7 +1751,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -1761,7 +1765,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -1775,7 +1779,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>78</v>
       </c>
@@ -1783,7 +1787,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
Mozny vypocet pri hospodarskem zisku 10^7
</commit_message>
<xml_diff>
--- a/Shareholding_EL-VY.xlsx
+++ b/Shareholding_EL-VY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/holec1/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E996D8-EAA6-834F-A7EE-B072834154A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E7C517-9DF4-B544-BB9C-6F03FD62D9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,14 +17,14 @@
     <sheet name="Seznam jmen" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="CelkovyNakladNarustMzdaDulZamestVerDob">Share_prog!$D$26</definedName>
-    <definedName name="CelkovyNakladNarustMzdaKlicZamestVerDob">Share_prog!$E$26</definedName>
-    <definedName name="CelkovyNakladNarustMzdaObchodZamestVerDob">Share_prog!$G$26</definedName>
-    <definedName name="CelkovyNakladNarustMzdaStratZamestVerDob">Share_prog!$F$26</definedName>
-    <definedName name="CelkovyNakladNarustMzdaZamestVerDob">Share_prog!$C$26</definedName>
-    <definedName name="CelyNakladShareDulZamest">Share_prog!$D$19</definedName>
-    <definedName name="CelyNakladShareKlicZamest">Share_prog!$D$17</definedName>
-    <definedName name="CelyNakladShareStratZamest">Share_prog!$D$21</definedName>
+    <definedName name="CelkovyNakladNarustMzdaDulZamestVerDob">Share_prog!$D$21</definedName>
+    <definedName name="CelkovyNakladNarustMzdaKlicZamestVerDob">Share_prog!$E$21</definedName>
+    <definedName name="CelkovyNakladNarustMzdaObchodZamestVerDob">Share_prog!$G$21</definedName>
+    <definedName name="CelkovyNakladNarustMzdaStratZamestVerDob">Share_prog!$F$21</definedName>
+    <definedName name="CelkovyNakladNarustMzdaZamestVerDob">Share_prog!$C$21</definedName>
+    <definedName name="CelyNakladShareDulZamest">Share_prog!$C$25</definedName>
+    <definedName name="CelyNakladShareKlicZamest">Share_prog!$C$23</definedName>
+    <definedName name="CelyNakladShareStratZamest">Share_prog!$C$27</definedName>
     <definedName name="CilMzdaDulZamest">Share_prog!$D$13</definedName>
     <definedName name="CilMzdaKlicZamest">Share_prog!$D$14</definedName>
     <definedName name="CilMzdaZamest">Share_prog!$D$12</definedName>
@@ -34,34 +34,34 @@
     <definedName name="HospVysledekProvoz">Share_prog!$C$7</definedName>
     <definedName name="MzdaPrumerCR">Share_prog!$D$11</definedName>
     <definedName name="MzdaZamest">Share_prog!#REF!</definedName>
-    <definedName name="NakladNarustMzdaDulZamestVerDob">Share_prog!$E$82</definedName>
-    <definedName name="NakladNarustMzdaKlicZamestVerDob">Share_prog!$E$87</definedName>
-    <definedName name="NakladNarustMzdaZamestVerDob">Share_prog!$E$77</definedName>
-    <definedName name="NakladObchodVerDob">Share_prog!$D$72</definedName>
-    <definedName name="NakladShareDulZamest">Share_prog!$C$51</definedName>
-    <definedName name="NakladShareKlicZamest">Share_prog!$C$47</definedName>
-    <definedName name="NakladShareStratZamest">Share_prog!$C$55</definedName>
+    <definedName name="NakladNarustMzdaDulZamestVerDob">Share_prog!$E$83</definedName>
+    <definedName name="NakladNarustMzdaKlicZamestVerDob">Share_prog!$E$88</definedName>
+    <definedName name="NakladNarustMzdaZamestVerDob">Share_prog!$E$78</definedName>
+    <definedName name="NakladObchodVerDob">Share_prog!$D$73</definedName>
+    <definedName name="NakladShareDulZamest">Share_prog!$C$52</definedName>
+    <definedName name="NakladShareKlicZamest">Share_prog!$C$48</definedName>
+    <definedName name="NakladShareStratZamest">Share_prog!$C$56</definedName>
     <definedName name="NarustMzdaDulZamest">Share_prog!#REF!</definedName>
-    <definedName name="NarustMzdaDulZamestZaklad">Share_prog!$D$81</definedName>
+    <definedName name="NarustMzdaDulZamestZaklad">Share_prog!$D$82</definedName>
     <definedName name="NarustMzdaKlicZamest">Share_prog!#REF!</definedName>
-    <definedName name="NarustMzdaKlicZamestZaklad">Share_prog!$D$86</definedName>
-    <definedName name="NarustMzdaZamest">Share_prog!$D$76</definedName>
-    <definedName name="PocetDulZamest">Share_prog!$C$19</definedName>
-    <definedName name="PocetKlicZamest">Share_prog!$C$17</definedName>
-    <definedName name="PocetObchod">Share_prog!$G$25</definedName>
-    <definedName name="PocetStratZamest">Share_prog!$C$21</definedName>
-    <definedName name="PocetZamest">Share_prog!$C$25</definedName>
+    <definedName name="NarustMzdaKlicZamestZaklad">Share_prog!$D$87</definedName>
+    <definedName name="NarustMzdaZamest">Share_prog!$D$77</definedName>
+    <definedName name="PocetDulZamest">Share_prog!$E$20</definedName>
+    <definedName name="PocetKlicZamest">Share_prog!$D$20</definedName>
+    <definedName name="PocetObchod">Share_prog!$G$20</definedName>
+    <definedName name="PocetStratZamest">Share_prog!$F$20</definedName>
+    <definedName name="PocetZamest">Share_prog!$C$20</definedName>
     <definedName name="ProcInvestice">Share_prog!$C$8</definedName>
     <definedName name="ProcMzdaDulZamest">Share_prog!#REF!</definedName>
     <definedName name="ProcMzdaKlicZamest">Share_prog!#REF!</definedName>
     <definedName name="ProcMzdaZamest">Share_prog!$D$15</definedName>
-    <definedName name="ProcShareDulZamest">Share_prog!$C$50</definedName>
-    <definedName name="ProcShareKlicZamest">Share_prog!$C$46</definedName>
-    <definedName name="ProcShareStartZamest">Share_prog!$C$54</definedName>
-    <definedName name="ShareDulZamest">Share_prog!$D$50</definedName>
-    <definedName name="ShareKlicZamest">Share_prog!$D$46</definedName>
-    <definedName name="ShareStratZamest">Share_prog!$D$54</definedName>
-    <definedName name="VernDoba">Share_prog!$C$28</definedName>
+    <definedName name="ProcShareDulZamest">Share_prog!$C$51</definedName>
+    <definedName name="ProcShareKlicZamest">Share_prog!$C$47</definedName>
+    <definedName name="ProcShareStartZamest">Share_prog!$C$55</definedName>
+    <definedName name="ShareDulZamest">Share_prog!$D$51</definedName>
+    <definedName name="ShareKlicZamest">Share_prog!$D$47</definedName>
+    <definedName name="ShareStratZamest">Share_prog!$D$55</definedName>
+    <definedName name="VernDoba">Share_prog!$C$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -86,9 +86,6 @@
     <t>Priklad realizace Shareholdingu se zamestnanci EL-VY</t>
   </si>
   <si>
-    <t>Hopodarsky vysledek 2021</t>
-  </si>
-  <si>
     <t>Maximalni hodnota sharovani</t>
   </si>
   <si>
@@ -348,6 +345,9 @@
   </si>
   <si>
     <t>Procenta celkova investice do lidi</t>
+  </si>
+  <si>
+    <t>Hopodarsky vysledek za rok</t>
   </si>
 </sst>
 </file>
@@ -739,10 +739,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z96"/>
+  <dimension ref="A1:Z97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -761,20 +761,20 @@
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
+      <c r="A5" s="22" t="s">
+        <v>88</v>
       </c>
       <c r="C5" s="2">
-        <v>4000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3">
         <v>0.2</v>
@@ -782,7 +782,7 @@
     </row>
     <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="2">
         <v>1000000</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="8" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="3">
         <v>0.05</v>
@@ -799,7 +799,7 @@
     <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="C9" s="2">
         <f xml:space="preserve"> HospVysledek * ProcInvestice</f>
-        <v>200000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -807,7 +807,7 @@
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="4">
         <v>42000</v>
@@ -815,7 +815,7 @@
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12">
         <v>0.4</v>
@@ -827,7 +827,7 @@
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13">
         <v>0.75</v>
@@ -839,7 +839,7 @@
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -851,465 +851,413 @@
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D16" s="4"/>
+      <c r="A16" s="1"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="15">
-        <v>4</v>
-      </c>
-      <c r="D17" s="16">
-        <f xml:space="preserve"> PocetKlicZamest * NakladShareKlicZamest</f>
-        <v>800000</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>14</v>
+        <v>5</v>
+      </c>
+      <c r="C17" s="1">
+        <v>5</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="16">
-        <f>D17 / VernDoba</f>
-        <v>160000</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="15">
+        <v>86</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="1">
+        <v>30</v>
+      </c>
+      <c r="D20" s="15">
         <v>4</v>
       </c>
-      <c r="D19" s="16">
-        <f xml:space="preserve"> PocetDulZamest * NakladShareDulZamest</f>
-        <v>560000</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="15">
+        <v>4</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21">
+        <f xml:space="preserve"> PocetZamest * NakladNarustMzdaZamestVerDob</f>
+        <v>3175200</v>
+      </c>
+      <c r="D21" s="4">
+        <f xml:space="preserve"> PocetDulZamest * NakladNarustMzdaDulZamestVerDob</f>
+        <v>793800</v>
+      </c>
+      <c r="E21">
+        <f xml:space="preserve"> PocetKlicZamest * NakladNarustMzdaKlicZamestVerDob</f>
+        <v>1058400</v>
+      </c>
+      <c r="F21">
+        <f xml:space="preserve"> PocetStratZamest * NakladNarustMzdaZamestVerDob</f>
+        <v>211680</v>
+      </c>
+      <c r="G21">
+        <f xml:space="preserve"> PocetObchod * NakladNarustMzdaZamestVerDob</f>
+        <v>211680</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="16">
+        <f xml:space="preserve"> PocetKlicZamest * NakladShareKlicZamest</f>
+        <v>2000000</v>
+      </c>
+      <c r="D23" s="22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="1"/>
+      <c r="C24" s="16">
+        <f>C23 / VernDoba</f>
+        <v>400000</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="16">
-        <f>D19 / VernDoba</f>
-        <v>112000</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="1">
-        <v>2</v>
-      </c>
-      <c r="D21" s="16">
-        <f xml:space="preserve"> PocetStratZamest * NakladShareStratZamest</f>
-        <v>1000000</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="16">
-        <f xml:space="preserve"> D21 / VernDoba</f>
-        <v>200000</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="22"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="F24" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="G24" s="22" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" s="1">
-        <v>30</v>
-      </c>
-      <c r="D25">
-        <f xml:space="preserve"> PocetDulZamest</f>
-        <v>4</v>
-      </c>
-      <c r="E25">
-        <f xml:space="preserve"> PocetKlicZamest</f>
-        <v>4</v>
-      </c>
-      <c r="F25">
-        <f xml:space="preserve"> PocetStratZamest</f>
-        <v>2</v>
-      </c>
-      <c r="G25">
-        <v>2</v>
+        <v>15</v>
+      </c>
+      <c r="C25" s="16">
+        <f xml:space="preserve"> PocetDulZamest * NakladShareDulZamest</f>
+        <v>1400000</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26">
-        <f xml:space="preserve"> PocetZamest * NakladNarustMzdaZamestVerDob</f>
-        <v>3175200</v>
-      </c>
-      <c r="D26" s="4">
-        <f xml:space="preserve"> PocetDulZamest * NakladNarustMzdaDulZamestVerDob</f>
-        <v>793800</v>
-      </c>
-      <c r="E26">
-        <f xml:space="preserve"> PocetKlicZamest * NakladNarustMzdaKlicZamestVerDob</f>
-        <v>1058400</v>
-      </c>
-      <c r="F26">
-        <f xml:space="preserve"> PocetStratZamest * NakladNarustMzdaZamestVerDob</f>
-        <v>211680</v>
-      </c>
-      <c r="G26">
-        <f xml:space="preserve"> PocetObchod * NakladNarustMzdaZamestVerDob</f>
-        <v>211680</v>
+      <c r="A26" s="1"/>
+      <c r="C26" s="16">
+        <f>C25 / VernDoba</f>
+        <v>280000</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="A28" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="1">
-        <v>5</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="A29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-    </row>
+      <c r="A27" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="16">
+        <f xml:space="preserve"> PocetStratZamest * NakladShareStratZamest</f>
+        <v>2500000</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="1"/>
+      <c r="C28" s="16">
+        <f xml:space="preserve"> C27 / VernDoba</f>
+        <v>500000</v>
+      </c>
+      <c r="D28" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="13" x14ac:dyDescent="0.15"/>
     <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="A30" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="F30" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="G30" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="H30" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="I30" s="22" t="s">
-        <v>88</v>
-      </c>
+      <c r="A30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="4">
+        <v>16</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="H31" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="I31" s="22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="13" x14ac:dyDescent="0.15">
+      <c r="A32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="4">
         <f xml:space="preserve"> VernDoba * (HospVysledek - HospProvoz - HospInvestice)</f>
-        <v>14000000</v>
-      </c>
-      <c r="D31" s="4">
+        <v>42500000</v>
+      </c>
+      <c r="D32" s="4">
         <f xml:space="preserve"> VernDoba * (HospVysledek - HospProvoz - HospInvestice) - CelyNakladShareKlicZamest - CelyNakladShareDulZamest - CelyNakladShareStratZamest</f>
-        <v>11640000</v>
-      </c>
-      <c r="E31" s="17">
+        <v>36600000</v>
+      </c>
+      <c r="E32" s="17">
         <f xml:space="preserve"> VernDoba * (HospVysledek - HospProvoz - HospInvestice) - (CelyNakladShareKlicZamest + CelyNakladShareDulZamest + CelyNakladShareStratZamest) - (CelkovyNakladNarustMzdaZamestVerDob + CelkovyNakladNarustMzdaDulZamestVerDob + CelkovyNakladNarustMzdaKlicZamestVerDob + CelkovyNakladNarustMzdaStratZamestVerDob + CelkovyNakladNarustMzdaObchodZamestVerDob) - PocetObchod * NakladObchodVerDob</f>
-        <v>5389240</v>
-      </c>
-      <c r="F31">
+        <v>30349240</v>
+      </c>
+      <c r="F32">
         <f xml:space="preserve"> (CelyNakladShareKlicZamest + CelyNakladShareDulZamest + CelyNakladShareStratZamest) / (HospVysledek * VernDoba) * 100</f>
         <v>11.799999999999999</v>
       </c>
-      <c r="G31">
+      <c r="G32">
         <f xml:space="preserve"> (CelkovyNakladNarustMzdaZamestVerDob + CelkovyNakladNarustMzdaDulZamestVerDob + CelkovyNakladNarustMzdaKlicZamestVerDob + CelkovyNakladNarustMzdaStratZamestVerDob + CelkovyNakladNarustMzdaObchodZamestVerDob) / (HospVysledek * VernDoba) * 100</f>
-        <v>27.253800000000002</v>
-      </c>
-      <c r="H31">
+        <v>10.901520000000001</v>
+      </c>
+      <c r="H32">
         <f xml:space="preserve"> PocetObchod * NakladObchodVerDob / (VernDoba * HospVysledek) * 100</f>
-        <v>4</v>
-      </c>
-      <c r="I31">
-        <f xml:space="preserve"> F31 + G31 + H31</f>
-        <v>43.053800000000003</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="13" x14ac:dyDescent="0.15">
-      <c r="A32" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="4">
-        <f t="shared" ref="C32" si="0">0.6*C31</f>
-        <v>8400000</v>
-      </c>
-      <c r="D32" s="4">
-        <f>0.6*D31</f>
-        <v>6984000</v>
-      </c>
-      <c r="E32">
-        <f>0.6*E31</f>
-        <v>3233544</v>
+        <v>1.6</v>
+      </c>
+      <c r="I32">
+        <f xml:space="preserve"> F32 + G32 + H32</f>
+        <v>24.301520000000004</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C33" s="4">
-        <f t="shared" ref="C33" si="1">0.2*C31</f>
-        <v>2800000</v>
+        <f t="shared" ref="C33" si="0">0.6*C32</f>
+        <v>25500000</v>
       </c>
       <c r="D33" s="4">
-        <f>0.2*D31</f>
-        <v>2328000</v>
+        <f>0.6*D32</f>
+        <v>21960000</v>
       </c>
       <c r="E33">
-        <f>0.2*E31</f>
-        <v>1077848</v>
+        <f>0.6*E32</f>
+        <v>18209544</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A34" s="17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C34" s="4">
-        <f t="shared" ref="C34:D34" si="2">0.2*C31</f>
-        <v>2800000</v>
+        <f t="shared" ref="C34" si="1">0.2*C32</f>
+        <v>8500000</v>
       </c>
       <c r="D34" s="4">
+        <f>0.2*D32</f>
+        <v>7320000</v>
+      </c>
+      <c r="E34">
+        <f>0.2*E32</f>
+        <v>6069848</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A35" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="4">
+        <f t="shared" ref="C35:D35" si="2">0.2*C32</f>
+        <v>8500000</v>
+      </c>
+      <c r="D35" s="4">
         <f t="shared" si="2"/>
-        <v>2328000</v>
-      </c>
-      <c r="E34">
-        <f>0.2*E31</f>
-        <v>1077848</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+        <v>7320000</v>
+      </c>
+      <c r="E35">
+        <f>0.2*E32</f>
+        <v>6069848</v>
+      </c>
     </row>
     <row r="36" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="23" t="s">
-        <v>81</v>
-      </c>
     </row>
     <row r="37" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A37" s="22" t="s">
-        <v>82</v>
-      </c>
+      <c r="A37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
-      <c r="E37">
-        <f xml:space="preserve"> NakladNarustMzdaZamestVerDob</f>
-        <v>105840</v>
+      <c r="E37" s="23" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A38" s="22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38">
-        <f xml:space="preserve"> NakladNarustMzdaDulZamestVerDob + NakladShareDulZamest</f>
-        <v>338450</v>
+        <f xml:space="preserve"> NakladNarustMzdaZamestVerDob</f>
+        <v>105840</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A39" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39">
-        <f xml:space="preserve"> NakladNarustMzdaKlicZamestVerDob + NakladShareKlicZamest</f>
-        <v>464600</v>
+        <f xml:space="preserve"> NakladNarustMzdaDulZamestVerDob + NakladShareDulZamest</f>
+        <v>548450</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A40" s="22" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40">
-        <f xml:space="preserve"> NakladNarustMzdaZamestVerDob + NakladObchodVerDob</f>
-        <v>505840</v>
+        <f xml:space="preserve"> NakladNarustMzdaKlicZamestVerDob + NakladShareKlicZamest</f>
+        <v>764600</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A41" s="22" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41">
-        <f xml:space="preserve"> NakladNarustMzdaZamestVerDob + NakladShareStratZamest</f>
-        <v>605840</v>
+        <f xml:space="preserve"> NakladNarustMzdaZamestVerDob + NakladObchodVerDob</f>
+        <v>505840</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A42" s="22"/>
+      <c r="A42" s="22" t="s">
+        <v>84</v>
+      </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
+      <c r="E42">
+        <f xml:space="preserve"> NakladNarustMzdaZamestVerDob + NakladShareStratZamest</f>
+        <v>1355840</v>
+      </c>
     </row>
     <row r="43" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A43" s="1"/>
+      <c r="A43" s="22"/>
       <c r="C43" s="1"/>
-      <c r="D43" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="E43">
-        <f xml:space="preserve"> E31 + PocetZamest * E37 + PocetDulZamest * E38 + PocetKlicZamest * E39 + PocetObchod * E40 + PocetStratZamest * E41</f>
-        <v>14000000</v>
-      </c>
+      <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A44" s="1"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
+      <c r="D44" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44">
+        <f xml:space="preserve"> E32 + PocetZamest * E38 + PocetDulZamest * E39 + PocetKlicZamest * E40 + PocetObchod * E41 + PocetStratZamest * E42</f>
+        <v>42500000</v>
+      </c>
     </row>
     <row r="45" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A45" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="4"/>
+      <c r="A45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A46" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="D46" s="2">
-        <f xml:space="preserve"> HospVysledek * ProcShareKlicZamest</f>
-        <v>40000</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="A46" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="D47" s="2">
+        <f xml:space="preserve"> HospVysledek * ProcShareKlicZamest</f>
+        <v>100000</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="4">
+        <f xml:space="preserve"> ShareKlicZamest * VernDoba</f>
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" ht="13" x14ac:dyDescent="0.15">
+      <c r="A49" s="1"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:26" ht="13" x14ac:dyDescent="0.15">
+      <c r="A50" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="4">
-        <f xml:space="preserve"> ShareKlicZamest * VernDoba</f>
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A48" s="1"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="1"/>
-    </row>
-    <row r="49" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A49" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" s="10"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="9"/>
-      <c r="L49" s="9"/>
-      <c r="M49" s="9"/>
-      <c r="N49" s="9"/>
-      <c r="O49" s="9"/>
-      <c r="P49" s="9"/>
-      <c r="Q49" s="9"/>
-      <c r="R49" s="9"/>
-      <c r="S49" s="9"/>
-      <c r="T49" s="9"/>
-      <c r="U49" s="9"/>
-      <c r="V49" s="9"/>
-      <c r="W49" s="9"/>
-      <c r="X49" s="9"/>
-      <c r="Y49" s="9"/>
-      <c r="Z49" s="9"/>
-    </row>
-    <row r="50" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A50" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="13">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="D50" s="11">
-        <f xml:space="preserve"> HospVysledek * ProcShareDulZamest</f>
-        <v>28000</v>
-      </c>
-      <c r="E50" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="C50" s="10"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="9"/>
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
       <c r="H50" s="9"/>
@@ -1334,15 +1282,19 @@
     </row>
     <row r="51" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="12" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B51" s="9"/>
-      <c r="C51" s="11">
-        <f xml:space="preserve"> ShareDulZamest * VernDoba</f>
-        <v>140000</v>
-      </c>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
+      <c r="C51" s="13">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="D51" s="11">
+        <f xml:space="preserve"> HospVysledek * ProcShareDulZamest</f>
+        <v>70000</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>9</v>
+      </c>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
@@ -1366,9 +1318,14 @@
       <c r="Z51" s="9"/>
     </row>
     <row r="52" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A52" s="12"/>
+      <c r="A52" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="B52" s="9"/>
-      <c r="C52" s="11"/>
+      <c r="C52" s="11">
+        <f xml:space="preserve"> ShareDulZamest * VernDoba</f>
+        <v>350000</v>
+      </c>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
       <c r="F52" s="9"/>
@@ -1394,9 +1351,12 @@
       <c r="Z52" s="9"/>
     </row>
     <row r="53" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A53" s="7" t="s">
-        <v>39</v>
-      </c>
+      <c r="A53" s="12"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="9"/>
       <c r="I53" s="9"/>
@@ -1419,18 +1379,8 @@
       <c r="Z53" s="9"/>
     </row>
     <row r="54" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A54" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C54" s="3">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="D54" s="4">
-        <f xml:space="preserve"> HospVysledek * ProcShareStartZamest</f>
-        <v>100000</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>10</v>
+      <c r="A54" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
@@ -1455,13 +1405,18 @@
     </row>
     <row r="55" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C55">
-        <f xml:space="preserve"> ShareStratZamest * VernDoba</f>
-        <v>500000</v>
-      </c>
-      <c r="D55" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="C55" s="3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D55" s="4">
+        <f xml:space="preserve"> HospVysledek * ProcShareStartZamest</f>
+        <v>250000</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
       <c r="I55" s="9"/>
@@ -1483,267 +1438,292 @@
       <c r="Y55" s="9"/>
       <c r="Z55" s="9"/>
     </row>
-    <row r="58" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A58" s="7" t="s">
-        <v>24</v>
-      </c>
+    <row r="56" spans="1:26" ht="13" x14ac:dyDescent="0.15">
+      <c r="A56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56">
+        <f xml:space="preserve"> ShareStratZamest * VernDoba</f>
+        <v>1250000</v>
+      </c>
+      <c r="D56" s="4"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="9"/>
+      <c r="O56" s="9"/>
+      <c r="P56" s="9"/>
+      <c r="Q56" s="9"/>
+      <c r="R56" s="9"/>
+      <c r="S56" s="9"/>
+      <c r="T56" s="9"/>
+      <c r="U56" s="9"/>
+      <c r="V56" s="9"/>
+      <c r="W56" s="9"/>
+      <c r="X56" s="9"/>
+      <c r="Y56" s="9"/>
+      <c r="Z56" s="9"/>
     </row>
     <row r="59" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A59" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" s="1"/>
+      <c r="A59" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="60" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4">
-        <v>5000000</v>
+        <v>25</v>
       </c>
     </row>
     <row r="62" spans="1:26" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26" ht="13" x14ac:dyDescent="0.15">
+      <c r="A63" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1">
+        <v>10</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1">
-        <v>10</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="64" spans="1:26" ht="13" x14ac:dyDescent="0.15">
-      <c r="A64" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A66" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4">
         <v>200000</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="B66" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18">
-        <v>0.2</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="B67" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D67" s="4">
-        <f>D65*(1-D66)</f>
-        <v>160000</v>
+        <v>31</v>
+      </c>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18">
+        <v>0.2</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="B68" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C68" s="19"/>
-      <c r="D68" s="19">
-        <v>0.05</v>
+        <v>32</v>
+      </c>
+      <c r="D68" s="4">
+        <f>D66*(1-D67)</f>
+        <v>160000</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="B69" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" s="19"/>
+      <c r="D69" s="19">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="B70" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C70" s="6"/>
+      <c r="D70" s="2">
+        <f>D68*D69</f>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B71" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C69" s="6"/>
-      <c r="D69" s="2">
-        <f>D67*D68</f>
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B70" s="1" t="s">
+    </row>
+    <row r="72" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A72" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A71" s="1" t="s">
+      <c r="C72" s="6"/>
+      <c r="D72" s="2">
+        <f>D70*D63</f>
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A73" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D73" s="16">
+        <f xml:space="preserve"> D72 * VernDoba</f>
+        <v>400000</v>
+      </c>
+      <c r="E73" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C71" s="6"/>
-      <c r="D71" s="2">
-        <f>D69*D62</f>
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A72" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="D72" s="16">
-        <f xml:space="preserve"> D71 * VernDoba</f>
-        <v>400000</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A75" s="7" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="76" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A76" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D76" s="2">
+      <c r="A76" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A77" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D77" s="2">
         <f xml:space="preserve"> CilMzdaZamest * ProcMzdaZamest</f>
         <v>252</v>
       </c>
-      <c r="E76" s="23" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A77" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C77" s="1">
+      <c r="E77" s="23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A78" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C78" s="1">
         <f xml:space="preserve"> VernDoba</f>
         <v>5</v>
       </c>
-      <c r="D77" s="4">
+      <c r="D78" s="4">
         <f xml:space="preserve"> CilMzdaZamest + VernDoba * (VernDoba + 1) / 2 * NarustMzdaZamest</f>
         <v>20580</v>
       </c>
-      <c r="E77">
+      <c r="E78">
         <f xml:space="preserve"> VernDoba * (VernDoba + 1)  * (VernDoba + 2) / 6 * NarustMzdaZamest * 12</f>
         <v>105840</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="C78" s="1">
+    <row r="79" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="C79" s="1">
         <f xml:space="preserve"> 2 * VernDoba</f>
         <v>10</v>
       </c>
-      <c r="D78" s="4">
+      <c r="D79" s="4">
         <f xml:space="preserve"> CilMzdaZamest + 2 * VernDoba * (2 * VernDoba + 1) / 2 * NarustMzdaZamest</f>
         <v>30660</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="C79" s="1"/>
-      <c r="D79" s="4"/>
-    </row>
     <row r="80" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A80" s="21" t="s">
-        <v>65</v>
-      </c>
       <c r="C80" s="1"/>
       <c r="D80" s="4"/>
     </row>
-    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" t="s">
-        <v>43</v>
-      </c>
-      <c r="D81">
+    <row r="81" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A81" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C81" s="1"/>
+      <c r="D81" s="4"/>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A82" t="s">
+        <v>42</v>
+      </c>
+      <c r="D82">
         <f xml:space="preserve"> CilMzdaDulZamest * ProcMzdaZamest</f>
         <v>472.5</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A82" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C82" s="1">
+    <row r="83" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A83" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C83" s="1">
         <f xml:space="preserve"> VernDoba</f>
         <v>5</v>
       </c>
-      <c r="D82" s="2">
+      <c r="D83" s="2">
         <f xml:space="preserve"> CilMzdaDulZamest + VernDoba * (VernDoba + 1) / 2 * NarustMzdaDulZamestZaklad</f>
         <v>38587.5</v>
       </c>
-      <c r="E82">
+      <c r="E83">
         <f xml:space="preserve"> VernDoba * (VernDoba + 1)  * (VernDoba + 2) / 6 * NarustMzdaDulZamestZaklad * 12</f>
         <v>198450</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A83" s="1"/>
-      <c r="C83" s="1">
+    <row r="84" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A84" s="1"/>
+      <c r="C84" s="1">
         <f xml:space="preserve"> 2 * VernDoba</f>
         <v>10</v>
       </c>
-      <c r="D83" s="2">
+      <c r="D84" s="2">
         <f xml:space="preserve"> CilMzdaDulZamest + 2 * VernDoba * (2 * VernDoba + 1) / 2 * NarustMzdaDulZamestZaklad</f>
         <v>57487.5</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="2"/>
-    </row>
     <row r="85" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A85" s="21" t="s">
-        <v>66</v>
-      </c>
+      <c r="A85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="2"/>
     </row>
     <row r="86" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A86" s="22" t="s">
-        <v>43</v>
+      <c r="A86" s="21" t="s">
+        <v>65</v>
       </c>
       <c r="C86" s="1"/>
-      <c r="D86" s="2">
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A87" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C87" s="1"/>
+      <c r="D87" s="2">
         <f xml:space="preserve"> CilMzdaKlicZamest * ProcMzdaZamest</f>
         <v>630</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A87" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C87" s="1">
+    <row r="88" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A88" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C88" s="1">
         <f xml:space="preserve"> VernDoba</f>
         <v>5</v>
       </c>
-      <c r="D87" s="2">
+      <c r="D88" s="2">
         <f xml:space="preserve"> CilMzdaKlicZamest + VernDoba * (VernDoba + 1) / 2 * NarustMzdaKlicZamestZaklad</f>
         <v>51450</v>
       </c>
-      <c r="E87">
+      <c r="E88">
         <f xml:space="preserve"> VernDoba * (VernDoba + 1)  * (VernDoba + 2) / 6 * NarustMzdaKlicZamestZaklad * 12</f>
         <v>264600</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A88" s="1"/>
-      <c r="C88" s="1">
+    <row r="89" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A89" s="1"/>
+      <c r="C89" s="1">
         <f xml:space="preserve"> 2 * VernDoba</f>
         <v>10</v>
       </c>
-      <c r="D88" s="2">
+      <c r="D89" s="2">
         <f xml:space="preserve"> CilMzdaKlicZamest + 2 * VernDoba * (2 * VernDoba + 1) / 2 * NarustMzdaKlicZamestZaklad</f>
         <v>76650</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A89" s="1"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="2"/>
     </row>
     <row r="90" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="1"/>
@@ -1755,14 +1735,19 @@
       <c r="C91" s="1"/>
       <c r="D91" s="2"/>
     </row>
-    <row r="93" spans="1:5" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="95" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A95" s="6"/>
-      <c r="D95" s="16"/>
-    </row>
-    <row r="96" spans="1:5" ht="14" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="A92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="2"/>
+    </row>
+    <row r="94" spans="1:5" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="96" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="6"/>
-      <c r="D96" s="20"/>
+      <c r="D96" s="16"/>
+    </row>
+    <row r="97" spans="1:4" ht="14" x14ac:dyDescent="0.2">
+      <c r="A97" s="6"/>
+      <c r="D97" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1786,60 +1771,60 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>46</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>